<commit_message>
last update before migrating to mySQL
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -718,7 +718,7 @@
       <c r="C14" s="14" t="n">
         <v>43754</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G14" s="8" t="inlineStr">
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="C15" s="14" t="n">
-        <v>43754</v>
+        <v>43756</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>1</v>
@@ -964,7 +964,12 @@
           <t>Aber das Schiff ist so gewaltig</t>
         </is>
       </c>
-      <c r="C27" s="14" t="n"/>
+      <c r="C27" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E27" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="G27" s="8" t="inlineStr">
         <is>
           <t>Pero el barco es tan enorme.</t>
@@ -1277,7 +1282,12 @@
           <t>Das ist eine Falle</t>
         </is>
       </c>
-      <c r="C43" s="14" t="n"/>
+      <c r="C43" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E43" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="G43" s="8" t="inlineStr">
         <is>
           <t>Eso es una trampa</t>
@@ -1295,7 +1305,12 @@
           <t>Er hat dieses Land verlassen</t>
         </is>
       </c>
-      <c r="C44" s="14" t="n"/>
+      <c r="C44" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E44" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="G44" s="8" t="inlineStr">
         <is>
           <t>Se fue de este pais</t>
@@ -1372,7 +1387,12 @@
           <t>Was tust du das</t>
         </is>
       </c>
-      <c r="C48" s="14" t="n"/>
+      <c r="C48" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E48" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="G48" s="8" t="inlineStr">
         <is>
           <t>Que estas haciendo</t>
@@ -1390,7 +1410,12 @@
           <t>Oh das könnte interessant werden</t>
         </is>
       </c>
-      <c r="C49" s="14" t="n"/>
+      <c r="C49" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E49" s="8" t="n">
+        <v>1</v>
+      </c>
       <c r="G49" s="8" t="inlineStr">
         <is>
           <t>Ohh, eso podría ser interesante</t>
@@ -1521,7 +1546,12 @@
           <t>Ja, kann ich mir vorstellen</t>
         </is>
       </c>
-      <c r="C56" s="14" t="n"/>
+      <c r="C56" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
       <c r="G56" s="8" t="inlineStr">
         <is>
           <t>Si me puedo imaginar</t>
@@ -1581,7 +1611,7 @@
         </is>
       </c>
       <c r="C59" s="14" t="n">
-        <v>43754</v>
+        <v>43756</v>
       </c>
       <c r="E59" s="8" t="n">
         <v>1</v>
@@ -1603,7 +1633,12 @@
           <t>Ja, auf jeden Fall</t>
         </is>
       </c>
-      <c r="C60" s="14" t="n"/>
+      <c r="C60" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
       <c r="G60" s="8" t="inlineStr">
         <is>
           <t>Si definitivamente</t>
@@ -1658,9 +1693,9 @@
         </is>
       </c>
       <c r="C63" s="14" t="n">
-        <v>43754</v>
-      </c>
-      <c r="E63" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E63" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="8" t="inlineStr">
@@ -1683,7 +1718,7 @@
       <c r="C64" s="14" t="n">
         <v>43754</v>
       </c>
-      <c r="E64" t="n">
+      <c r="E64" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G64" s="8" t="inlineStr">
@@ -1804,7 +1839,7 @@
         </is>
       </c>
       <c r="C70" s="14" t="n">
-        <v>43754</v>
+        <v>43756</v>
       </c>
       <c r="E70" s="8" t="n">
         <v>1</v>
@@ -1827,7 +1862,7 @@
         </is>
       </c>
       <c r="C71" s="14" t="n">
-        <v>43754</v>
+        <v>43756</v>
       </c>
       <c r="E71" s="8" t="n">
         <v>1</v>
@@ -2061,7 +2096,12 @@
           <t>Das Risiko müssen wir eingehen.</t>
         </is>
       </c>
-      <c r="C83" s="14" t="n"/>
+      <c r="C83" s="14" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1</v>
+      </c>
       <c r="G83" s="8" t="inlineStr">
         <is>
           <t>Tenemos que arriesgarnos.</t>
@@ -2146,7 +2186,7 @@
       <c r="C87" s="14" t="n">
         <v>43754</v>
       </c>
-      <c r="E87" t="n">
+      <c r="E87" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G87" s="8" t="inlineStr">
@@ -2187,7 +2227,7 @@
       <c r="C89" s="16" t="n">
         <v>43754</v>
       </c>
-      <c r="E89" t="n">
+      <c r="E89" s="8" t="n">
         <v>1</v>
       </c>
       <c r="G89" s="8" t="inlineStr">
@@ -2278,9 +2318,9 @@
         </is>
       </c>
       <c r="C94" s="16" t="n">
-        <v>43754</v>
-      </c>
-      <c r="E94" t="n">
+        <v>43756</v>
+      </c>
+      <c r="E94" s="8" t="n">
         <v>2</v>
       </c>
       <c r="G94" s="8" t="inlineStr">

</xml_diff>